<commit_message>
update calling code and population
</commit_message>
<xml_diff>
--- a/inst/population.xlsx
+++ b/inst/population.xlsx
@@ -1571,6 +1571,9 @@
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D9" s="4">
+        <v>15753.0</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -5624,6 +5627,9 @@
       <c r="C168" s="1" t="s">
         <v>163</v>
       </c>
+      <c r="D168" s="4">
+        <v>5483450.0</v>
+      </c>
       <c r="E168" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>